<commit_message>
Add 10 new potential leads to dashboard - Updated potential-leads-table with new leads from Exotel calls including ABDULQADIR JAFFAR POONAWALA, VINAYA GANESH KADAM, and 8 others - Total leads now: 100 (90 existing + 10 new) - All new leads marked as PENDING CALLBACK with Exotel call notes
</commit_message>
<xml_diff>
--- a/interested_customers_20250923_230841.xlsx
+++ b/interested_customers_20250923_230841.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c84bafc70a8a41f3/Documents/Outbound caller/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shlok\Downloads\Realeaste dash (clone of the OG)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_28ABBC54A5BBF83BB9CA87C8F9E57605C5065856" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B526812D-BB18-4D30-98A0-AC171013A9B8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D34769-25E9-4939-8A89-F05125C137C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:K51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,6 +2692,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>